<commit_message>
PWA: manifest, service worker, iconos
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\Trabajos\Raven.Net\buzzerlive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2EE692-6402-4C40-A503-8B810E1FED3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49178175-7C46-4DDD-91AE-80E699C709D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t xml:space="preserve">Obras: </t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>al apretar Partidos en Vivo, entra en todos los partidos</t>
+  </si>
+  <si>
+    <t>falta un salir de la visualizacion del partido en espectador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falta un "suspender" partido para que el partido quede guardado todos los datos al momento de la suspension </t>
+  </si>
+  <si>
+    <t>al momento de agregar una falta, deberia abrirse un menu flotante que indique que tipo de falta es (personal, tecnica, antideportiva, descalificadora)</t>
+  </si>
+  <si>
+    <t>en caso de sumar 2 faltas tecnicas, 2 faltas antideportivas o 1 falta tecn y 1 desc, el jugador queda descalificado de ese partido debe aparecer un GD</t>
+  </si>
+  <si>
+    <t>el jugador que hace 5 faltas esta bien que no pueda tener mas acciones, pero debe poder hacer sustitucion para que entre otro jugador suplente</t>
+  </si>
+  <si>
+    <t>al momento de cargar jugadores nuevos se tiene que poder marcar al mismo como jugador Refuerzo, el cual va a tener reglas especiales en cuanto a la cantidad de cuartos que puede jugar</t>
+  </si>
+  <si>
+    <t>al iniciar el juego, pero antes de elegir a los 5 titulares, los dos equipos deberian poder elegir a los 12 jugadores citados para el juego</t>
   </si>
 </sst>
 </file>
@@ -455,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4361B226-EBF9-4690-AABC-691FAC8212B9}">
-  <dimension ref="A2:B16"/>
+  <dimension ref="A2:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,16 +528,25 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -528,9 +558,44 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: PWA iconos y service worker
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\Trabajos\Raven.Net\buzzerlive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49178175-7C46-4DDD-91AE-80E699C709D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BB8E17-EE24-4D10-84B4-F441A850B85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">Obras: </t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>al iniciar el juego, pero antes de elegir a los 5 titulares, los dos equipos deberian poder elegir a los 12 jugadores citados para el juego</t>
+  </si>
+  <si>
+    <t>en los logacciones deberia aparecer que terminó el cuarto y al momento de hacer la falta debe informar, tipo de falta, si da lanzamientos y cantidad de faltas de ese jugador</t>
+  </si>
+  <si>
+    <t>tambien deben aparecer las correcciones</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4361B226-EBF9-4690-AABC-691FAC8212B9}">
-  <dimension ref="A2:B22"/>
+  <dimension ref="A2:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,6 +604,16 @@
         <v>21</v>
       </c>
     </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
arreglo de bugs generales
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\Trabajos\Raven.Net\buzzerlive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BB8E17-EE24-4D10-84B4-F441A850B85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6959D92-B3DA-4AEF-BBFA-BE9884164886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t xml:space="preserve">Obras: </t>
   </si>
@@ -83,18 +83,6 @@
     <t>los partidos deberian estar ordenados desde el mas proximo al mas lejano y despues los ya jugados</t>
   </si>
   <si>
-    <t>al apretar Partidos en Vivo, entra en todos los partidos</t>
-  </si>
-  <si>
-    <t>falta un salir de la visualizacion del partido en espectador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">falta un "suspender" partido para que el partido quede guardado todos los datos al momento de la suspension </t>
-  </si>
-  <si>
-    <t>al momento de agregar una falta, deberia abrirse un menu flotante que indique que tipo de falta es (personal, tecnica, antideportiva, descalificadora)</t>
-  </si>
-  <si>
     <t>en caso de sumar 2 faltas tecnicas, 2 faltas antideportivas o 1 falta tecn y 1 desc, el jugador queda descalificado de ese partido debe aparecer un GD</t>
   </si>
   <si>
@@ -104,13 +92,46 @@
     <t>al momento de cargar jugadores nuevos se tiene que poder marcar al mismo como jugador Refuerzo, el cual va a tener reglas especiales en cuanto a la cantidad de cuartos que puede jugar</t>
   </si>
   <si>
-    <t>al iniciar el juego, pero antes de elegir a los 5 titulares, los dos equipos deberian poder elegir a los 12 jugadores citados para el juego</t>
-  </si>
-  <si>
     <t>en los logacciones deberia aparecer que terminó el cuarto y al momento de hacer la falta debe informar, tipo de falta, si da lanzamientos y cantidad de faltas de ese jugador</t>
   </si>
   <si>
-    <t>tambien deben aparecer las correcciones</t>
+    <t>los numeros de camiseta tienen que poder modificarse antes de iniciar el juego</t>
+  </si>
+  <si>
+    <t>falta un salir de la visualizacion del partido en espectador para volver a la pagina anterior o al menu o a los partidos (decidilo vos)</t>
+  </si>
+  <si>
+    <t>falta un "suspender" partido para que el partido quede guardado todos los datos al momento de la suspension, al momento de suspenderse debe abrir un cuadro de observaciones explicando el por qué de la suspension</t>
+  </si>
+  <si>
+    <t>al momento de agregar una falta, deberia abrirse un menu flotante que indique que tipo de falta es (personal, tecnica, antideportiva, descalificadora) y (salvo la falta tecnica) marcar la cantidad de lanzamientos que debe hacer 0,1,2,3.</t>
+  </si>
+  <si>
+    <t>al iniciar el juego, pero antes de elegir a los 5 titulares, los dos equipos deberian poder elegir a los 12 jugadores citados para el juego. Ya que puede haber equipos que tienen mas de 12 jugadores anotados para jugar el torneo</t>
+  </si>
+  <si>
+    <t>tambien deben aparecer las correcciones (descuentos)</t>
+  </si>
+  <si>
+    <t>el entrenador tambien debe aparecer en algun lugar (podria ser debajo de los 5 titulares, el cual tambien puede recibir falta tecnica o descalificatoria</t>
+  </si>
+  <si>
+    <t>al apretar Partidos en Vivo, entra en todos los partidos, deberia entrar directamente a los partidos en vivo</t>
+  </si>
+  <si>
+    <t>en el index, los partidos en vivo y los ultimos resultados no estan apareciendo</t>
+  </si>
+  <si>
+    <t>para qué sirve el boton Cargar Partido si me lleva a la seccion Partidos? Al igual que el boton Partidos. Es para que despues use el administrador de torneos?</t>
+  </si>
+  <si>
+    <t>falta un salir de la carga  del partido en el planiller para volver a la pagina anterior o al menu o a los partidos (decidilo vos)</t>
+  </si>
+  <si>
+    <t>si el jugador está con cero faltas se le pueden seguir descontando y las sacas de las falta de equipo</t>
+  </si>
+  <si>
+    <t>en el celular hay que arreglar la adaptabilidad y ver por qué en la app no gira la pantalla, ya que es mucho mas comodo usarlo de esta forma</t>
   </si>
 </sst>
 </file>
@@ -482,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4361B226-EBF9-4690-AABC-691FAC8212B9}">
-  <dimension ref="A2:B24"/>
+  <dimension ref="A2:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,60 +579,172 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>24</v>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixes: descontar tipos, 1T+1A=expulsión, modal continuar, tracking faltas
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\Trabajos\Raven.Net\buzzerlive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D228EC31-D98D-41F7-A28C-23222B439A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9126EA87-57CC-4CF3-AA86-C2D2E3561AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t xml:space="preserve">Obras: </t>
   </si>
@@ -509,7 +509,7 @@
   <dimension ref="A2:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="B19" sqref="B19:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,127 +635,86 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1</v>
+      <c r="A20" t="s">
+        <v>29</v>
       </c>
       <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>9</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>3</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 12 citados, faltas entrenador, log expandido
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\Trabajos\Raven.Net\buzzerlive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9126EA87-57CC-4CF3-AA86-C2D2E3561AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F06DDF-3C30-4410-991B-143DEC096937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t xml:space="preserve">Obras: </t>
   </si>
@@ -92,9 +92,6 @@
     <t>al momento de cargar jugadores nuevos se tiene que poder marcar al mismo como jugador Refuerzo, el cual va a tener reglas especiales en cuanto a la cantidad de cuartos que puede jugar</t>
   </si>
   <si>
-    <t>en los logacciones deberia aparecer que terminó el cuarto y al momento de hacer la falta debe informar, tipo de falta, si da lanzamientos y cantidad de faltas de ese jugador</t>
-  </si>
-  <si>
     <t>los numeros de camiseta tienen que poder modificarse antes de iniciar el juego</t>
   </si>
   <si>
@@ -131,10 +128,16 @@
     <t>si el jugador está con cero faltas se le pueden seguir descontando y las sacas de las falta de equipo</t>
   </si>
   <si>
-    <t>en el celular hay que arreglar la adaptabilidad y ver por qué en la app no gira la pantalla, ya que es mucho mas comodo usarlo de esta forma</t>
-  </si>
-  <si>
     <t>un jugador descalificado y/o con 5 faltas, no tiene que poder ingresar de nuevo al quinteto de juego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en los logacciones deberia aparecer que terminó el cuarto </t>
+  </si>
+  <si>
+    <t>en logacc al momento de hacer la falta debe informar, tipo de falta, si da lanzamientos y cantidad de faltas de ese jugador</t>
+  </si>
+  <si>
+    <t>en el celular hay que arreglar la adaptabilidad y ver por qué en la app no gira la pantalla, ya que es mucho mas comodo usarlo de esta forma se podria hacer que al momento de entrar en el partido en modo planillero se gire automaticamente</t>
   </si>
 </sst>
 </file>
@@ -506,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4361B226-EBF9-4690-AABC-691FAC8212B9}">
-  <dimension ref="A2:B36"/>
+  <dimension ref="A2:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B25"/>
+      <selection activeCell="A33" sqref="A33:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,7 +599,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -604,7 +607,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -612,7 +615,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -628,7 +631,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -636,7 +639,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -644,7 +647,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -652,7 +655,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -660,7 +663,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -668,7 +671,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -676,45 +679,59 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 6: Arquitectura multi-tenant
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\Trabajos\Raven.Net\buzzerlive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1442D816-5782-4C8E-A4AA-8900EF008111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21783648-B3C1-401B-8213-45E7071A7FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t xml:space="preserve">San Lorenzo: </t>
   </si>
   <si>
-    <t xml:space="preserve"> Boca: </t>
-  </si>
-  <si>
     <t>aeefd149-3ce7-401a-9773-5ee480f6e81a</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>los elegidos para el partido deben ser al menos 5, no forzar a que marque 12 jugadores, si algun equipo no llega a 5 jugadores, se debe aclarar al empezar el partido que "El Equipo X no completa el minimo de jugadores necesarios"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boca: </t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4361B226-EBF9-4690-AABC-691FAC8212B9}">
   <dimension ref="A2:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -558,223 +558,223 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 7,8,9: admin, planiller, storage
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\Trabajos\Raven.Net\buzzerlive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21783648-B3C1-401B-8213-45E7071A7FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEB1927-9CE3-431A-8349-983BCAE8AEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{F7E6239F-32DC-4A16-944D-FA69FA16E448}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t xml:space="preserve">Obras: </t>
   </si>
@@ -153,16 +153,42 @@
   </si>
   <si>
     <t xml:space="preserve">Boca: </t>
+  </si>
+  <si>
+    <t>sebastian.ravenna@gmail.com</t>
+  </si>
+  <si>
+    <t>admin1234</t>
+  </si>
+  <si>
+    <t>SuperAdmin</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>rchevi@hotmail.com</t>
+  </si>
+  <si>
+    <t>chevi1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,13 +211,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -524,15 +553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4361B226-EBF9-4690-AABC-691FAC8212B9}">
-  <dimension ref="A2:B44"/>
+  <dimension ref="A2:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -540,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -548,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -556,7 +585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -564,15 +593,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -580,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -588,7 +637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -596,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -604,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -612,7 +661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -620,7 +669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -778,7 +827,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{85EBB12E-78E3-47BA-90D6-9A4803D64F35}"/>
+    <hyperlink ref="H9" r:id="rId2" xr:uid="{23EDF104-8F3E-4477-8151-2B0DA4D15476}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>